<commit_message>
Some more Spain data
</commit_message>
<xml_diff>
--- a/a-place-for-salvador-allende/countries/Spain_1.xlsx
+++ b/a-place-for-salvador-allende/countries/Spain_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onemsci-my.sharepoint.com/personal/glo_canonoy_msci_com/Documents/03 Training/datasets-of-interest/a-place-for-salvador-allende/countries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="139" documentId="11_116901F3F613C8A64D9379BF459AD9D24CB67BE2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEDCFEDB-61DC-45E1-9084-212176568CAA}"/>
+  <xr:revisionPtr revIDLastSave="409" documentId="11_116901F3F613C8A64D9379BF459AD9D24CB67BE2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E79650A-A0F4-45CF-8D5B-3871C03EB2EF}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Y$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Y$34</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="237">
   <si>
     <t>id</t>
   </si>
@@ -196,15 +196,6 @@
   </si>
   <si>
     <t>Galicia</t>
-  </si>
-  <si>
-    <t>Conella de Llobregat, Castuera</t>
-  </si>
-  <si>
-    <t>Atarle</t>
-  </si>
-  <si>
-    <t>Móstoles, Henares, San Sebastián, Coslada</t>
   </si>
   <si>
     <t>Asturias</t>
@@ -494,13 +485,318 @@
     <t>https://goo.gl/maps/gwgszxHTweSoZbrv8</t>
   </si>
   <si>
-    <t>Cubelles, Vigo, Ingenio, Asturias, Santiago de Compostela, Fortuna</t>
-  </si>
-  <si>
     <t>A Salvador Allende</t>
   </si>
   <si>
-    <t>Granada, Montcada, Alicante, Valencia, Toledo,  Alcoy, Algeciras, Almansa, Arrecife, Posadas</t>
+    <t>Sigan ustedes sabiendo que, mucho más temprano que tarde, de nuevo abrirán las grandes alamedas por donde pase el hombre libre, para construir una sociedad mejor.
+Salvador Allende Gossens
+11 de Septiembre de 1973
+Ayuntamiento de Gijón
+Obra de Mónica Bunster
+Réplica de la instalada en Palmilla (Chile)
+Gijón, Mayo de 1999</t>
+  </si>
+  <si>
+    <t>Avenida de Salvador Allende</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/3CqTudJLv3rRXKtA6</t>
+  </si>
+  <si>
+    <t>Bajo Llobregat</t>
+  </si>
+  <si>
+    <t>Cornellà de Llobregat</t>
+  </si>
+  <si>
+    <t>la Gavarra</t>
+  </si>
+  <si>
+    <t>08940</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/551625663</t>
+  </si>
+  <si>
+    <t>Granada</t>
+  </si>
+  <si>
+    <t>Comarca de la Vega de Granada</t>
+  </si>
+  <si>
+    <t>Atarfe</t>
+  </si>
+  <si>
+    <t>Santa Amalia</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/550263249</t>
+  </si>
+  <si>
+    <t>openstreetmap</t>
+  </si>
+  <si>
+    <t>Al presidente de Chile Salvador Allende por la libertad. Atarfe 1992. "Colocado en un trance histórico, pagaré con mi vida la lealtad del pueblo." Salvador Allende. Septiembre 1973</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/iFvZRAxkkawBfHCT6</t>
+  </si>
+  <si>
+    <t>Móstoles</t>
+  </si>
+  <si>
+    <t>San Sebastián</t>
+  </si>
+  <si>
+    <t>Coslada</t>
+  </si>
+  <si>
+    <t>Parque de Salvador Allende</t>
+  </si>
+  <si>
+    <t>Villafontana II</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/32012075</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/uKQPCy1mmCMT1eBD9</t>
+  </si>
+  <si>
+    <t>Salvador Allende Parkea</t>
+  </si>
+  <si>
+    <t>Autonomous Community of the Basque Country</t>
+  </si>
+  <si>
+    <t>Gipuzkoa</t>
+  </si>
+  <si>
+    <t>Donostialdea</t>
+  </si>
+  <si>
+    <t>Mirakruz - Bidebieta</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/217198782</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/64SwajnNtehwq73x6?coh=178573&amp;entry=tt</t>
+  </si>
+  <si>
+    <t>eu, es, en, fr</t>
+  </si>
+  <si>
+    <t>Memoriaren Lekuak
+Lugares de la Memoria
+Salvador Allende Park
+Scene of executions
+Bidebieta firing range, 1936.
+The firing range of Bidebieta, scene of multiple executions after the capture of the city (13/09/1936) by the coup troops, was located on this land. Around 400 people are currently estimated to have been shot in San Sebastián in the context of the Francoist Repression between 1936 and 1945.</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/28505387</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/WGeKtPU2YU8wGJdG6</t>
+  </si>
+  <si>
+    <t>Cubelles</t>
+  </si>
+  <si>
+    <t>Vigo</t>
+  </si>
+  <si>
+    <t>Ingenio</t>
+  </si>
+  <si>
+    <t>Santiago de Compostela</t>
+  </si>
+  <si>
+    <t>Fortuna</t>
+  </si>
+  <si>
+    <t>Toledo</t>
+  </si>
+  <si>
+    <t>Alcoy</t>
+  </si>
+  <si>
+    <t>Algeciras</t>
+  </si>
+  <si>
+    <t>Almansa</t>
+  </si>
+  <si>
+    <t>Arrecife</t>
+  </si>
+  <si>
+    <t>Posadas</t>
+  </si>
+  <si>
+    <t>Calle Salvador Allende</t>
+  </si>
+  <si>
+    <t>Peligros</t>
+  </si>
+  <si>
+    <t>Monteluz</t>
+  </si>
+  <si>
+    <t>18210</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/129324725</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/oMHse5jSRb9dGQWb9</t>
+  </si>
+  <si>
+    <t>Parc Salvador Allende</t>
+  </si>
+  <si>
+    <t>Vallés Occidental</t>
+  </si>
+  <si>
+    <t>Montcada i Reixac</t>
+  </si>
+  <si>
+    <t>Montcada Nova</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/453500065</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/djWpvB6arNFoEgb6A?coh=178573&amp;entry=tt</t>
+  </si>
+  <si>
+    <t>Castile-La Mancha</t>
+  </si>
+  <si>
+    <t>Talavera</t>
+  </si>
+  <si>
+    <t>Talavera de la Reina</t>
+  </si>
+  <si>
+    <t>San Jerónimo</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/650379497</t>
+  </si>
+  <si>
+    <t>Montes de Toledo</t>
+  </si>
+  <si>
+    <t>Urda</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/214486907</t>
+  </si>
+  <si>
+    <t>Torrijos</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/365006471</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/qWed3bGEkYVo9YEu6</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/CDm4dncQjQJHfzXz7</t>
+  </si>
+  <si>
+    <t>Calle Voluntarios de Toledo</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/jh8ftYy82vUd4G167?coh=178573&amp;entry=tt</t>
+  </si>
+  <si>
+    <t>Carrer Salvador Allende</t>
+  </si>
+  <si>
+    <t>Alicante</t>
+  </si>
+  <si>
+    <t>La Hoya de Alcoy</t>
+  </si>
+  <si>
+    <t>Santa Rosa</t>
+  </si>
+  <si>
+    <t>03802</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/55218876</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/3MvXdjUtpRjtx9Fn7?coh=178573&amp;entry=tt</t>
+  </si>
+  <si>
+    <t>Carrer Salvador Allende
+President de Xile
+1970-1973</t>
+  </si>
+  <si>
+    <t>ca</t>
+  </si>
+  <si>
+    <t>Campo de Gibraltar</t>
+  </si>
+  <si>
+    <t>Urbanización Parque Bolonia</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/267056639</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/SkP8RxmWehrP5wWv5</t>
+  </si>
+  <si>
+    <t>Calle Salvador Allende
+Político Chileno (1908-1973)</t>
+  </si>
+  <si>
+    <t>Albacete</t>
+  </si>
+  <si>
+    <t>https://www.openstreetmap.org/way/571083259</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/abTfhQjfrmbsnuae8</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/9cAzsKdB4vSEJMvm7</t>
+  </si>
+  <si>
+    <t>Canary Islands</t>
+  </si>
+  <si>
+    <t>Las Palmas</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/5ZJFtdXr44tKmoFJA</t>
+  </si>
+  <si>
+    <t>Rúa de Salvador Allende</t>
+  </si>
+  <si>
+    <t>Pontevedra</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/NX3xPQ4BGnV1wDL17</t>
+  </si>
+  <si>
+    <t>Rúa do Presidente Salvador Allende</t>
+  </si>
+  <si>
+    <t>https://goo.gl/maps/HrpfMDbq7MtLUdpa6</t>
+  </si>
+  <si>
+    <t>Region of Murcia</t>
+  </si>
+  <si>
+    <t>Avenida Salvador Allende</t>
   </si>
 </sst>
 </file>
@@ -581,13 +877,14 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -927,10 +1224,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y20"/>
+  <dimension ref="A1:Y34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1029,16 +1326,16 @@
         <v>38</v>
       </c>
       <c r="G2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="L2">
         <v>39.229927600000003</v>
@@ -1053,19 +1350,19 @@
         <v>7</v>
       </c>
       <c r="Q2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="V2">
         <v>1</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
@@ -1085,13 +1382,13 @@
         <v>39</v>
       </c>
       <c r="G3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L3">
         <v>40.5376756</v>
@@ -1106,30 +1403,30 @@
         <v>6</v>
       </c>
       <c r="Q3" t="s">
+        <v>114</v>
+      </c>
+      <c r="R3" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="R3" s="3" t="s">
-        <v>120</v>
-      </c>
       <c r="S3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="V3">
         <v>1</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
@@ -1144,19 +1441,19 @@
         <v>40</v>
       </c>
       <c r="G4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="K4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L4">
         <v>41.439136300000001</v>
@@ -1174,25 +1471,25 @@
         <v>11</v>
       </c>
       <c r="Q4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="V4">
         <v>1</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
@@ -1209,16 +1506,16 @@
         <v>37</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G5" t="s">
         <v>41</v>
       </c>
       <c r="H5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="L5">
         <v>43.355326849999997</v>
@@ -1233,24 +1530,24 @@
         <v>9</v>
       </c>
       <c r="Q5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="V5">
         <v>1</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C6" t="s">
         <v>33</v>
@@ -1262,16 +1559,16 @@
         <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G6" t="s">
         <v>42</v>
       </c>
       <c r="H6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L6">
         <v>43.517951449999998</v>
@@ -1282,25 +1579,34 @@
       <c r="N6">
         <v>1999</v>
       </c>
+      <c r="O6">
+        <v>5</v>
+      </c>
       <c r="Q6" t="s">
-        <v>86</v>
+        <v>85</v>
+      </c>
+      <c r="R6" t="s">
+        <v>138</v>
+      </c>
+      <c r="S6" t="s">
+        <v>109</v>
       </c>
       <c r="V6">
         <v>1</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C7" t="s">
         <v>32</v>
@@ -1315,16 +1621,16 @@
         <v>39</v>
       </c>
       <c r="G7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H7" t="s">
         <v>43</v>
       </c>
       <c r="I7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K7">
         <v>28054</v>
@@ -1345,30 +1651,30 @@
         <v>7</v>
       </c>
       <c r="Q7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="S7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="V7">
         <v>1</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="Y7" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C8" t="s">
         <v>33</v>
@@ -1383,16 +1689,16 @@
         <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I8" t="s">
         <v>44</v>
       </c>
       <c r="J8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="K8">
         <v>43850</v>
@@ -1413,13 +1719,13 @@
         <v>11</v>
       </c>
       <c r="Q8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="V8">
         <v>0</v>
       </c>
       <c r="Y8" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
@@ -1439,13 +1745,13 @@
         <v>39</v>
       </c>
       <c r="G9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L9">
         <v>40.5375364</v>
@@ -1460,25 +1766,25 @@
         <v>6</v>
       </c>
       <c r="Q9" t="s">
+        <v>114</v>
+      </c>
+      <c r="R9" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="R9" s="3" t="s">
-        <v>120</v>
-      </c>
       <c r="S9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="V9">
         <v>1</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X9" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="Y9" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
@@ -1498,19 +1804,19 @@
         <v>40</v>
       </c>
       <c r="G10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="K10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="L10">
         <v>41.606675799999998</v>
@@ -1522,19 +1828,19 @@
         <v>1998</v>
       </c>
       <c r="Q10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="V10">
         <v>1</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Y10" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
@@ -1554,16 +1860,16 @@
         <v>40</v>
       </c>
       <c r="G11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H11" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="I11" t="s">
         <v>45</v>
       </c>
       <c r="J11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K11">
         <v>43491</v>
@@ -1584,25 +1890,31 @@
         <v>16</v>
       </c>
       <c r="Q11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="S11" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="V11">
         <v>1</v>
       </c>
       <c r="X11" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="Y11" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>183</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
       <c r="D12" t="s">
         <v>36</v>
       </c>
@@ -1610,7 +1922,28 @@
         <v>37</v>
       </c>
       <c r="F12" t="s">
-        <v>142</v>
+        <v>48</v>
+      </c>
+      <c r="G12" t="s">
+        <v>146</v>
+      </c>
+      <c r="H12" t="s">
+        <v>147</v>
+      </c>
+      <c r="I12" t="s">
+        <v>184</v>
+      </c>
+      <c r="J12" t="s">
+        <v>185</v>
+      </c>
+      <c r="K12" t="s">
+        <v>186</v>
+      </c>
+      <c r="L12">
+        <v>37.229588700000001</v>
+      </c>
+      <c r="M12">
+        <v>-3.6307174999999998</v>
       </c>
       <c r="N12">
         <v>2007</v>
@@ -1622,21 +1955,27 @@
         <v>18</v>
       </c>
       <c r="Q12" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="V12">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="W12" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="X12" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="Y12" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>29</v>
+        <v>189</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
         <v>36</v>
@@ -1645,28 +1984,25 @@
         <v>37</v>
       </c>
       <c r="F13" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G13" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="H13" t="s">
-        <v>66</v>
+        <v>190</v>
       </c>
       <c r="I13" t="s">
-        <v>71</v>
+        <v>191</v>
       </c>
       <c r="J13" t="s">
-        <v>76</v>
-      </c>
-      <c r="K13" t="s">
-        <v>83</v>
+        <v>192</v>
       </c>
       <c r="L13">
-        <v>43.319771099999997</v>
+        <v>41.488509999999998</v>
       </c>
       <c r="M13">
-        <v>-8.3764702999999994</v>
+        <v>2.18621</v>
       </c>
       <c r="N13">
         <v>2007</v>
@@ -1678,22 +2014,28 @@
         <v>18</v>
       </c>
       <c r="Q13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="V13">
         <v>1</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>96</v>
+        <v>193</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>137</v>
+        <v>194</v>
       </c>
       <c r="Y13" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
       <c r="D14" t="s">
         <v>36</v>
       </c>
@@ -1701,7 +2043,28 @@
         <v>37</v>
       </c>
       <c r="F14" t="s">
-        <v>47</v>
+        <v>195</v>
+      </c>
+      <c r="G14" t="s">
+        <v>177</v>
+      </c>
+      <c r="H14" t="s">
+        <v>196</v>
+      </c>
+      <c r="I14" t="s">
+        <v>197</v>
+      </c>
+      <c r="J14" t="s">
+        <v>198</v>
+      </c>
+      <c r="K14">
+        <v>45600</v>
+      </c>
+      <c r="L14">
+        <v>39.961350000000003</v>
+      </c>
+      <c r="M14">
+        <v>-4.8255400000000002</v>
       </c>
       <c r="N14">
         <v>2007</v>
@@ -1713,16 +2076,28 @@
         <v>18</v>
       </c>
       <c r="Q14" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="V14">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="W14" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="X14" s="2" t="s">
+        <v>205</v>
       </c>
       <c r="Y14" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>183</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
       <c r="D15" t="s">
         <v>36</v>
       </c>
@@ -1730,7 +2105,22 @@
         <v>37</v>
       </c>
       <c r="F15" t="s">
-        <v>140</v>
+        <v>195</v>
+      </c>
+      <c r="G15" t="s">
+        <v>177</v>
+      </c>
+      <c r="H15" t="s">
+        <v>200</v>
+      </c>
+      <c r="I15" t="s">
+        <v>201</v>
+      </c>
+      <c r="L15">
+        <v>39.413800000000002</v>
+      </c>
+      <c r="M15">
+        <v>-3.7234500000000001</v>
       </c>
       <c r="N15">
         <v>2007</v>
@@ -1742,18 +2132,27 @@
         <v>18</v>
       </c>
       <c r="Q15" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="V15">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="W15" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="X15" s="2" t="s">
+        <v>206</v>
       </c>
       <c r="Y15" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>183</v>
+      </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s">
         <v>36</v>
@@ -1762,30 +2161,57 @@
         <v>37</v>
       </c>
       <c r="F16" t="s">
-        <v>48</v>
+        <v>195</v>
+      </c>
+      <c r="G16" t="s">
+        <v>177</v>
+      </c>
+      <c r="H16" t="s">
+        <v>203</v>
+      </c>
+      <c r="K16">
+        <v>45500</v>
+      </c>
+      <c r="L16">
+        <v>39.986899999999999</v>
+      </c>
+      <c r="M16">
+        <v>-4.2808400000000004</v>
       </c>
       <c r="N16">
-        <v>2007</v>
+        <v>2018</v>
       </c>
       <c r="O16">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="P16">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="Q16" t="s">
-        <v>87</v>
+        <v>151</v>
+      </c>
+      <c r="U16" t="s">
+        <v>207</v>
       </c>
       <c r="V16">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="W16" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="X16" s="2" t="s">
+        <v>208</v>
       </c>
       <c r="Y16" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>209</v>
+      </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s">
         <v>36</v>
@@ -1794,7 +2220,28 @@
         <v>37</v>
       </c>
       <c r="F17" t="s">
-        <v>49</v>
+        <v>38</v>
+      </c>
+      <c r="G17" t="s">
+        <v>210</v>
+      </c>
+      <c r="H17" t="s">
+        <v>211</v>
+      </c>
+      <c r="I17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J17" t="s">
+        <v>212</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="L17">
+        <v>38.695999999999998</v>
+      </c>
+      <c r="M17">
+        <v>-0.48238999999999999</v>
       </c>
       <c r="N17">
         <v>2007</v>
@@ -1806,21 +2253,33 @@
         <v>18</v>
       </c>
       <c r="Q17" t="s">
-        <v>87</v>
+        <v>84</v>
+      </c>
+      <c r="S17" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="T17" t="s">
+        <v>217</v>
       </c>
       <c r="V17">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="W17" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="X17" s="2" t="s">
+        <v>215</v>
       </c>
       <c r="Y17" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>30</v>
+        <v>113</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s">
         <v>36</v>
@@ -1829,28 +2288,28 @@
         <v>37</v>
       </c>
       <c r="F18" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="G18" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="H18" t="s">
-        <v>67</v>
+        <v>218</v>
       </c>
       <c r="I18" t="s">
-        <v>72</v>
+        <v>179</v>
       </c>
       <c r="J18" t="s">
-        <v>77</v>
-      </c>
-      <c r="K18" t="s">
-        <v>84</v>
+        <v>219</v>
+      </c>
+      <c r="K18">
+        <v>11202</v>
       </c>
       <c r="L18">
-        <v>40.290276499999997</v>
+        <v>36.134619999999998</v>
       </c>
       <c r="M18">
-        <v>-3.798069870771331</v>
+        <v>-5.4523099999999998</v>
       </c>
       <c r="N18">
         <v>2007</v>
@@ -1862,22 +2321,34 @@
         <v>18</v>
       </c>
       <c r="Q18" t="s">
-        <v>87</v>
+        <v>84</v>
+      </c>
+      <c r="S18" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="T18" t="s">
+        <v>109</v>
       </c>
       <c r="V18">
         <v>1</v>
       </c>
       <c r="W18" s="2" t="s">
-        <v>97</v>
+        <v>220</v>
       </c>
       <c r="X18" s="2" t="s">
-        <v>138</v>
+        <v>221</v>
       </c>
       <c r="Y18" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
       <c r="D19" t="s">
         <v>36</v>
       </c>
@@ -1885,7 +2356,19 @@
         <v>37</v>
       </c>
       <c r="F19" t="s">
-        <v>50</v>
+        <v>195</v>
+      </c>
+      <c r="G19" t="s">
+        <v>223</v>
+      </c>
+      <c r="H19" t="s">
+        <v>180</v>
+      </c>
+      <c r="L19">
+        <v>38.86786</v>
+      </c>
+      <c r="M19">
+        <v>-1.09619</v>
       </c>
       <c r="N19">
         <v>2007</v>
@@ -1897,18 +2380,24 @@
         <v>18</v>
       </c>
       <c r="Q19" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="V19">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="W19" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="X19" s="2" t="s">
+        <v>225</v>
       </c>
       <c r="Y19" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>31</v>
+        <v>113</v>
       </c>
       <c r="C20" t="s">
         <v>32</v>
@@ -1920,28 +2409,22 @@
         <v>37</v>
       </c>
       <c r="F20" t="s">
-        <v>51</v>
+        <v>227</v>
       </c>
       <c r="G20" t="s">
-        <v>59</v>
+        <v>228</v>
       </c>
       <c r="H20" t="s">
-        <v>68</v>
-      </c>
-      <c r="I20" t="s">
-        <v>73</v>
-      </c>
-      <c r="J20" t="s">
-        <v>78</v>
-      </c>
-      <c r="K20" t="s">
-        <v>85</v>
+        <v>181</v>
+      </c>
+      <c r="K20">
+        <v>35500</v>
       </c>
       <c r="L20">
-        <v>36.686493200000001</v>
+        <v>28.966757091767398</v>
       </c>
       <c r="M20">
-        <v>-6.1395356000000003</v>
+        <v>-13.5553765146192</v>
       </c>
       <c r="N20">
         <v>2007</v>
@@ -1953,23 +2436,739 @@
         <v>18</v>
       </c>
       <c r="Q20" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="V20">
         <v>1</v>
       </c>
-      <c r="W20" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="X20" s="2" t="s">
-        <v>139</v>
+        <v>226</v>
       </c>
       <c r="Y20" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" t="s">
+        <v>182</v>
+      </c>
+      <c r="N21">
+        <v>2007</v>
+      </c>
+      <c r="O21">
+        <v>2</v>
+      </c>
+      <c r="P21">
+        <v>18</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>84</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H22" t="s">
+        <v>63</v>
+      </c>
+      <c r="I22" t="s">
+        <v>68</v>
+      </c>
+      <c r="J22" t="s">
+        <v>73</v>
+      </c>
+      <c r="K22" t="s">
+        <v>80</v>
+      </c>
+      <c r="L22">
+        <v>43.319771099999997</v>
+      </c>
+      <c r="M22">
+        <v>-8.3764702999999994</v>
+      </c>
+      <c r="N22">
+        <v>2007</v>
+      </c>
+      <c r="O22">
+        <v>2</v>
+      </c>
+      <c r="P22">
+        <v>18</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>84</v>
+      </c>
+      <c r="V22">
+        <v>1</v>
+      </c>
+      <c r="W22" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="X22" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y22" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" t="s">
+        <v>51</v>
+      </c>
+      <c r="H23" t="s">
+        <v>141</v>
+      </c>
+      <c r="I23" t="s">
+        <v>142</v>
+      </c>
+      <c r="J23" t="s">
+        <v>143</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="L23">
+        <v>41.356788999999999</v>
+      </c>
+      <c r="M23">
+        <v>2.075485</v>
+      </c>
+      <c r="N23">
+        <v>2007</v>
+      </c>
+      <c r="O23">
+        <v>2</v>
+      </c>
+      <c r="P23">
+        <v>18</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>84</v>
+      </c>
+      <c r="V23">
+        <v>1</v>
+      </c>
+      <c r="W23" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="X23" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y23" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" t="s">
+        <v>172</v>
+      </c>
+      <c r="N24">
+        <v>2007</v>
+      </c>
+      <c r="O24">
+        <v>2</v>
+      </c>
+      <c r="P24">
+        <v>18</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>84</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>230</v>
+      </c>
+      <c r="C25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" t="s">
+        <v>231</v>
+      </c>
+      <c r="H25" t="s">
+        <v>173</v>
+      </c>
+      <c r="K25">
+        <v>36210</v>
+      </c>
+      <c r="L25">
+        <v>42.218725622078601</v>
+      </c>
+      <c r="M25">
+        <v>-8.7372137121920694</v>
+      </c>
+      <c r="N25">
+        <v>2007</v>
+      </c>
+      <c r="O25">
+        <v>2</v>
+      </c>
+      <c r="P25">
+        <v>18</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>84</v>
+      </c>
+      <c r="V25">
+        <v>1</v>
+      </c>
+      <c r="X25" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="Y25" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" t="s">
+        <v>174</v>
+      </c>
+      <c r="N26">
+        <v>2007</v>
+      </c>
+      <c r="O26">
+        <v>2</v>
+      </c>
+      <c r="P26">
+        <v>18</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>84</v>
+      </c>
+      <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>233</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" t="s">
+        <v>46</v>
+      </c>
+      <c r="G27" t="s">
+        <v>55</v>
+      </c>
+      <c r="H27" t="s">
+        <v>175</v>
+      </c>
+      <c r="K27">
+        <v>15705</v>
+      </c>
+      <c r="L27">
+        <v>42.881865280720298</v>
+      </c>
+      <c r="M27">
+        <v>-8.5491510724775104</v>
+      </c>
+      <c r="N27">
+        <v>2007</v>
+      </c>
+      <c r="O27">
+        <v>2</v>
+      </c>
+      <c r="P27">
+        <v>18</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>84</v>
+      </c>
+      <c r="V27">
+        <v>1</v>
+      </c>
+      <c r="X27" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="Y27" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>236</v>
+      </c>
+      <c r="C28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F28" t="s">
+        <v>235</v>
+      </c>
+      <c r="G28" t="s">
+        <v>176</v>
+      </c>
+      <c r="L28">
+        <v>38.179723988982602</v>
+      </c>
+      <c r="M28">
+        <v>-1.12729404939768</v>
+      </c>
+      <c r="N28">
+        <v>2007</v>
+      </c>
+      <c r="O28">
+        <v>2</v>
+      </c>
+      <c r="P28">
+        <v>18</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>84</v>
+      </c>
+      <c r="V28">
+        <v>1</v>
+      </c>
+      <c r="X28" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="Y28" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29" t="s">
+        <v>48</v>
+      </c>
+      <c r="G29" t="s">
+        <v>146</v>
+      </c>
+      <c r="H29" t="s">
+        <v>147</v>
+      </c>
+      <c r="I29" t="s">
+        <v>148</v>
+      </c>
+      <c r="J29" t="s">
+        <v>149</v>
+      </c>
+      <c r="L29">
+        <v>37.228879999999997</v>
+      </c>
+      <c r="M29">
+        <v>-3.6839300000000001</v>
+      </c>
+      <c r="N29">
+        <v>1992</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>85</v>
+      </c>
+      <c r="R29" t="s">
+        <v>152</v>
+      </c>
+      <c r="S29" t="s">
         <v>109</v>
       </c>
+      <c r="V29">
+        <v>1</v>
+      </c>
+      <c r="W29" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="X29" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y29" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>157</v>
+      </c>
+      <c r="C30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" t="s">
+        <v>36</v>
+      </c>
+      <c r="E30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" t="s">
+        <v>39</v>
+      </c>
+      <c r="G30" t="s">
+        <v>50</v>
+      </c>
+      <c r="H30" t="s">
+        <v>154</v>
+      </c>
+      <c r="I30" t="s">
+        <v>158</v>
+      </c>
+      <c r="L30">
+        <v>40.326099999999997</v>
+      </c>
+      <c r="M30">
+        <v>-3.8505600000000002</v>
+      </c>
+      <c r="N30">
+        <v>2007</v>
+      </c>
+      <c r="O30">
+        <v>2</v>
+      </c>
+      <c r="P30">
+        <v>18</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>84</v>
+      </c>
+      <c r="V30">
+        <v>1</v>
+      </c>
+      <c r="W30" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="X30" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y30" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>161</v>
+      </c>
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" t="s">
+        <v>36</v>
+      </c>
+      <c r="E31" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" t="s">
+        <v>162</v>
+      </c>
+      <c r="G31" t="s">
+        <v>163</v>
+      </c>
+      <c r="H31" t="s">
+        <v>164</v>
+      </c>
+      <c r="I31" t="s">
+        <v>155</v>
+      </c>
+      <c r="J31" t="s">
+        <v>165</v>
+      </c>
+      <c r="L31">
+        <v>43.324399999999997</v>
+      </c>
+      <c r="M31">
+        <v>-1.94347</v>
+      </c>
+      <c r="N31">
+        <v>2007</v>
+      </c>
+      <c r="O31">
+        <v>2</v>
+      </c>
+      <c r="P31">
+        <v>18</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>84</v>
+      </c>
+      <c r="R31" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="S31" t="s">
+        <v>168</v>
+      </c>
+      <c r="V31">
+        <v>1</v>
+      </c>
+      <c r="W31" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="X31" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y31" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>157</v>
+      </c>
+      <c r="C32" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" t="s">
+        <v>37</v>
+      </c>
+      <c r="F32" t="s">
+        <v>39</v>
+      </c>
+      <c r="G32" t="s">
+        <v>50</v>
+      </c>
+      <c r="H32" t="s">
+        <v>156</v>
+      </c>
+      <c r="L32">
+        <v>40.4289147</v>
+      </c>
+      <c r="M32">
+        <v>-3.546082771422018</v>
+      </c>
+      <c r="N32">
+        <v>2007</v>
+      </c>
+      <c r="O32">
+        <v>2</v>
+      </c>
+      <c r="P32">
+        <v>18</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>84</v>
+      </c>
+      <c r="V32">
+        <v>1</v>
+      </c>
+      <c r="W32" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="X32" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="Y32" s="2"/>
+    </row>
+    <row r="33" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" t="s">
+        <v>37</v>
+      </c>
+      <c r="F33" t="s">
+        <v>39</v>
+      </c>
+      <c r="G33" t="s">
+        <v>50</v>
+      </c>
+      <c r="H33" t="s">
+        <v>64</v>
+      </c>
+      <c r="I33" t="s">
+        <v>69</v>
+      </c>
+      <c r="J33" t="s">
+        <v>74</v>
+      </c>
+      <c r="K33" t="s">
+        <v>81</v>
+      </c>
+      <c r="L33">
+        <v>40.290276499999997</v>
+      </c>
+      <c r="M33">
+        <v>-3.798069870771331</v>
+      </c>
+      <c r="N33">
+        <v>2007</v>
+      </c>
+      <c r="O33">
+        <v>2</v>
+      </c>
+      <c r="P33">
+        <v>18</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>84</v>
+      </c>
+      <c r="V33">
+        <v>1</v>
+      </c>
+      <c r="W33" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="X33" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y33" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" t="s">
+        <v>37</v>
+      </c>
+      <c r="F34" t="s">
+        <v>48</v>
+      </c>
+      <c r="G34" t="s">
+        <v>56</v>
+      </c>
+      <c r="H34" t="s">
+        <v>65</v>
+      </c>
+      <c r="I34" t="s">
+        <v>70</v>
+      </c>
+      <c r="J34" t="s">
+        <v>75</v>
+      </c>
+      <c r="K34" t="s">
+        <v>82</v>
+      </c>
+      <c r="L34">
+        <v>36.686493200000001</v>
+      </c>
+      <c r="M34">
+        <v>-6.1395356000000003</v>
+      </c>
+      <c r="N34">
+        <v>2007</v>
+      </c>
+      <c r="O34">
+        <v>2</v>
+      </c>
+      <c r="P34">
+        <v>18</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>84</v>
+      </c>
+      <c r="V34">
+        <v>1</v>
+      </c>
+      <c r="W34" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="X34" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y34" s="2" t="s">
+        <v>106</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Y20" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:Y34" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="W2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="Y2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
@@ -1989,32 +3188,64 @@
     <hyperlink ref="Y10" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
     <hyperlink ref="Y11" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
     <hyperlink ref="Y12" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="W13" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="Y13" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="Y14" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="Y15" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="Y16" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="Y17" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="W18" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="Y18" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="Y19" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="W20" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="Y20" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="W7" r:id="rId30" xr:uid="{AFEDFFE1-75A2-4FE8-8505-50B8F8F94163}"/>
-    <hyperlink ref="X7" r:id="rId31" xr:uid="{DFEB62A7-6284-4BFD-9814-C067918E791B}"/>
-    <hyperlink ref="X2" r:id="rId32" xr:uid="{D2342D3D-57C3-437B-9D7B-31603EAFC89F}"/>
-    <hyperlink ref="X3" r:id="rId33" xr:uid="{3996A3CD-0C76-4071-9CEC-815329C8B2B8}"/>
-    <hyperlink ref="X9" r:id="rId34" xr:uid="{5AAB36D1-CDE7-41FF-9966-29C2D5F48392}"/>
-    <hyperlink ref="X4" r:id="rId35" xr:uid="{1E5DA217-96B0-4009-A1DB-685A90C52DF1}"/>
-    <hyperlink ref="X5" r:id="rId36" xr:uid="{C39757D8-319A-4F7C-A341-5B7FEDB52262}"/>
-    <hyperlink ref="X6" r:id="rId37" xr:uid="{D9D738A0-C0D6-45BC-A594-303A4F4DDFF4}"/>
-    <hyperlink ref="X10" r:id="rId38" xr:uid="{557AC0E3-E864-433F-A9F6-4F5A6A0A3D6F}"/>
-    <hyperlink ref="X11" r:id="rId39" xr:uid="{FB6AA678-F141-4314-9D32-4A6CFACF2420}"/>
-    <hyperlink ref="X13" r:id="rId40" xr:uid="{52EB4870-411D-4921-9AF7-FB5E2D2BB980}"/>
-    <hyperlink ref="X18" r:id="rId41" xr:uid="{B4DDDEDA-1FAD-4399-A180-858DA65FD8FE}"/>
-    <hyperlink ref="X20" r:id="rId42" xr:uid="{E1F95D0E-9C3D-461B-860D-DEAC930D7A7B}"/>
+    <hyperlink ref="W22" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="Y22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="Y23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="Y24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="Y29" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="Y30" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="W33" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="Y33" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="W34" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="Y34" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="W7" r:id="rId29" xr:uid="{AFEDFFE1-75A2-4FE8-8505-50B8F8F94163}"/>
+    <hyperlink ref="X7" r:id="rId30" xr:uid="{DFEB62A7-6284-4BFD-9814-C067918E791B}"/>
+    <hyperlink ref="X2" r:id="rId31" xr:uid="{D2342D3D-57C3-437B-9D7B-31603EAFC89F}"/>
+    <hyperlink ref="X3" r:id="rId32" xr:uid="{3996A3CD-0C76-4071-9CEC-815329C8B2B8}"/>
+    <hyperlink ref="X9" r:id="rId33" xr:uid="{5AAB36D1-CDE7-41FF-9966-29C2D5F48392}"/>
+    <hyperlink ref="X4" r:id="rId34" xr:uid="{1E5DA217-96B0-4009-A1DB-685A90C52DF1}"/>
+    <hyperlink ref="X5" r:id="rId35" xr:uid="{C39757D8-319A-4F7C-A341-5B7FEDB52262}"/>
+    <hyperlink ref="X6" r:id="rId36" xr:uid="{D9D738A0-C0D6-45BC-A594-303A4F4DDFF4}"/>
+    <hyperlink ref="X10" r:id="rId37" xr:uid="{557AC0E3-E864-433F-A9F6-4F5A6A0A3D6F}"/>
+    <hyperlink ref="X11" r:id="rId38" xr:uid="{FB6AA678-F141-4314-9D32-4A6CFACF2420}"/>
+    <hyperlink ref="X22" r:id="rId39" xr:uid="{52EB4870-411D-4921-9AF7-FB5E2D2BB980}"/>
+    <hyperlink ref="X33" r:id="rId40" xr:uid="{B4DDDEDA-1FAD-4399-A180-858DA65FD8FE}"/>
+    <hyperlink ref="X34" r:id="rId41" xr:uid="{E1F95D0E-9C3D-461B-860D-DEAC930D7A7B}"/>
+    <hyperlink ref="X23" r:id="rId42" xr:uid="{89FDE718-3E05-4478-BBE8-1F95867ADCD1}"/>
+    <hyperlink ref="W23" r:id="rId43" xr:uid="{9D59BBA4-3450-4659-A081-8C43D5849878}"/>
+    <hyperlink ref="W29" r:id="rId44" xr:uid="{0EB7BC04-FCC0-4FC8-9139-BE30DAB17E5A}"/>
+    <hyperlink ref="X29" r:id="rId45" xr:uid="{FECFBAE7-4B43-41A4-8F91-71705C097AAA}"/>
+    <hyperlink ref="W30" r:id="rId46" xr:uid="{2268C24B-BC14-4814-9FDD-1153A26338C5}"/>
+    <hyperlink ref="X30" r:id="rId47" xr:uid="{01E31A95-7237-4BE1-9210-25D8D4965D1D}"/>
+    <hyperlink ref="W31" r:id="rId48" xr:uid="{1F7B6239-AF9D-4211-B2ED-C5CAEB09960B}"/>
+    <hyperlink ref="X31" r:id="rId49" xr:uid="{816F0BB3-BAB0-4130-B6AC-3B55A06AA805}"/>
+    <hyperlink ref="Y31" r:id="rId50" xr:uid="{2DC170A8-5387-46B1-800A-B299D2ECAF7D}"/>
+    <hyperlink ref="W32" r:id="rId51" xr:uid="{D6289EEB-6F5D-49B7-BC59-416A906164F3}"/>
+    <hyperlink ref="X32" r:id="rId52" xr:uid="{89BE85DF-0CD6-4863-B082-BC7777407376}"/>
+    <hyperlink ref="Y25:Y28" r:id="rId53" display="http://www.abacq.org/calle/index.php?2007/02/18/20-espana" xr:uid="{A2CC6D8B-9F8B-49E0-8BB9-807156F30F51}"/>
+    <hyperlink ref="W12" r:id="rId54" xr:uid="{A8A638B6-71A7-4485-A2F8-46EA642EDAC7}"/>
+    <hyperlink ref="X12" r:id="rId55" xr:uid="{FCE4D0FC-FA52-4299-8917-00A45E217B03}"/>
+    <hyperlink ref="W13" r:id="rId56" xr:uid="{2BDD448A-9E06-4C15-A51A-34BCF334CCAB}"/>
+    <hyperlink ref="X13" r:id="rId57" xr:uid="{DC401386-827F-4555-910F-B5EB4D78D99C}"/>
+    <hyperlink ref="W14" r:id="rId58" xr:uid="{98F93056-41EA-430C-BC63-28FA4BF42F4E}"/>
+    <hyperlink ref="W15" r:id="rId59" xr:uid="{725309EA-BA8C-4DD3-AD53-3E9850F9FD08}"/>
+    <hyperlink ref="W16" r:id="rId60" xr:uid="{1BFCA764-4722-4D54-B9B3-B2E8527DF16E}"/>
+    <hyperlink ref="X14" r:id="rId61" xr:uid="{B8CFFB1C-E159-4AA8-8A85-6BD29AC15FF0}"/>
+    <hyperlink ref="X15" r:id="rId62" xr:uid="{8969FE68-9764-4D87-AE66-4A290F1AE1F1}"/>
+    <hyperlink ref="X16" r:id="rId63" xr:uid="{DE8ADFC2-9C43-48BA-8BC3-499D71B880FC}"/>
+    <hyperlink ref="W17" r:id="rId64" xr:uid="{A7DF1E47-23C1-4243-A85D-98C3409D4E20}"/>
+    <hyperlink ref="X17" r:id="rId65" xr:uid="{FCE18412-1915-4625-A9C4-5A19F0413D27}"/>
+    <hyperlink ref="W18" r:id="rId66" xr:uid="{15581B38-041A-471D-97A6-5FB17731EDD6}"/>
+    <hyperlink ref="X18" r:id="rId67" xr:uid="{71F64CB3-4744-42F4-B44C-0E67C027BBD6}"/>
+    <hyperlink ref="W19" r:id="rId68" xr:uid="{6A612C7E-8988-4E45-8BDC-F1DB4DF60ACE}"/>
+    <hyperlink ref="X19" r:id="rId69" xr:uid="{E5D6CFDB-7E4D-4332-BEC4-648053AB7AFA}"/>
+    <hyperlink ref="X20" r:id="rId70" xr:uid="{4A7BC952-193D-4701-BB48-5AABBAE730EA}"/>
+    <hyperlink ref="X25" r:id="rId71" xr:uid="{4774BC45-7792-4618-A075-8437D48986AA}"/>
+    <hyperlink ref="X27" r:id="rId72" xr:uid="{F5E5B515-678F-4D98-A474-8AA8B5729612}"/>
+    <hyperlink ref="X28" r:id="rId73" xr:uid="{257363AC-8F76-4B32-832E-D4A9D3BE6952}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId43"/>
+  <pageSetup orientation="portrait" r:id="rId74"/>
+  <legacyDrawing r:id="rId75"/>
 </worksheet>
 </file>
</xml_diff>